<commit_message>
add function to add task
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -2,10 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C68EF0-C107-4230-B865-BEE3D179523A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="true" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Number of task</t>
   </si>
@@ -48,12 +47,27 @@
   <si>
     <t>count solved</t>
   </si>
+  <si>
+    <t>30-01-25</t>
+  </si>
+  <si>
+    <t>9999</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>9998</t>
+  </si>
+  <si>
+    <t>9997</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,16 +99,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -102,7 +116,7 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -115,7 +129,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme 2007 - 2010">
   <a:themeElements>
     <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
@@ -403,21 +417,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="130.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="17.5546875"/>
+    <col customWidth="true" max="2" min="2" width="10.109375"/>
+    <col customWidth="true" max="3" min="3" width="130.5546875"/>
+    <col customWidth="true" max="4" min="4" width="11"/>
+    <col customWidth="true" max="5" min="5" width="10"/>
+    <col customWidth="true" max="6" min="6" width="15.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -435,7 +449,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>45683</v>
       </c>
@@ -453,7 +467,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>45564</v>
       </c>
@@ -471,7 +485,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>45565</v>
       </c>
@@ -489,7 +503,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>45682</v>
       </c>
@@ -507,7 +521,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>45566</v>
       </c>
@@ -525,7 +539,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>45685</v>
       </c>
@@ -543,7 +557,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>45685</v>
       </c>
@@ -561,7 +575,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>45685</v>
       </c>
@@ -579,7 +593,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>45685</v>
       </c>
@@ -597,7 +611,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>45686</v>
       </c>
@@ -615,7 +629,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>45685</v>
       </c>
@@ -633,7 +647,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>45568</v>
       </c>
@@ -651,7 +665,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>45569</v>
       </c>
@@ -669,7 +683,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>45686</v>
       </c>
@@ -687,7 +701,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>45686</v>
       </c>
@@ -705,7 +719,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>45569</v>
       </c>
@@ -723,7 +737,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>45569</v>
       </c>
@@ -741,7 +755,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>45573</v>
       </c>
@@ -759,7 +773,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>45640</v>
       </c>
@@ -777,7 +791,7 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>45582</v>
       </c>
@@ -795,7 +809,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
         <v>45582</v>
       </c>
@@ -813,7 +827,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
         <v>45582</v>
       </c>
@@ -831,7 +845,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
         <v>45582</v>
       </c>
@@ -849,7 +863,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>45582</v>
       </c>
@@ -867,7 +881,7 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>45582</v>
       </c>
@@ -885,7 +899,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>45585</v>
       </c>
@@ -903,7 +917,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
         <v>45592</v>
       </c>
@@ -921,7 +935,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
         <v>45593</v>
       </c>
@@ -939,7 +953,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
         <v>45593</v>
       </c>
@@ -957,7 +971,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
         <v>45593</v>
       </c>
@@ -975,7 +989,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
         <v>45593</v>
       </c>
@@ -993,7 +1007,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
         <v>45593</v>
       </c>
@@ -1011,7 +1025,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
         <v>45593</v>
       </c>
@@ -1029,7 +1043,7 @@
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
         <v>45594</v>
       </c>
@@ -1047,7 +1061,7 @@
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
         <v>45595</v>
       </c>
@@ -1065,7 +1079,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
         <v>45333</v>
       </c>
@@ -1083,7 +1097,7 @@
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
         <v>45603</v>
       </c>
@@ -1101,7 +1115,7 @@
       </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
         <v>45604</v>
       </c>
@@ -1119,7 +1133,7 @@
       </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
         <v>45604</v>
       </c>
@@ -1137,7 +1151,7 @@
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
         <v>45607</v>
       </c>
@@ -1155,7 +1169,7 @@
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
         <v>45610</v>
       </c>
@@ -1173,7 +1187,7 @@
       </c>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
         <v>45610</v>
       </c>
@@ -1191,7 +1205,7 @@
       </c>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
         <v>45682</v>
       </c>
@@ -1209,7 +1223,7 @@
       </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
         <v>45682</v>
       </c>
@@ -1227,7 +1241,7 @@
       </c>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
         <v>45683</v>
       </c>
@@ -1245,7 +1259,7 @@
       </c>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
         <v>45614</v>
       </c>
@@ -1263,7 +1277,7 @@
       </c>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
         <v>45615</v>
       </c>
@@ -1281,7 +1295,7 @@
       </c>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
         <v>45618</v>
       </c>
@@ -1299,7 +1313,7 @@
       </c>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
         <v>45618</v>
       </c>
@@ -1317,7 +1331,7 @@
       </c>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
         <v>45618</v>
       </c>
@@ -1335,7 +1349,7 @@
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6">
       <c r="A52" s="2">
         <v>45619</v>
       </c>
@@ -1353,7 +1367,7 @@
       </c>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6">
       <c r="A53" s="2">
         <v>45619</v>
       </c>
@@ -1371,7 +1385,7 @@
       </c>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6">
       <c r="A54" s="2">
         <v>45681</v>
       </c>
@@ -1389,7 +1403,7 @@
       </c>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6">
       <c r="A55" s="2">
         <v>45678</v>
       </c>
@@ -1407,7 +1421,7 @@
       </c>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6">
       <c r="A56" s="2">
         <v>45620</v>
       </c>
@@ -1425,7 +1439,7 @@
       </c>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6">
       <c r="A57" s="2">
         <v>45620</v>
       </c>
@@ -1443,7 +1457,7 @@
       </c>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6">
       <c r="A58" s="2">
         <v>45621</v>
       </c>
@@ -1461,7 +1475,7 @@
       </c>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6">
       <c r="A59" s="2">
         <v>45621</v>
       </c>
@@ -1479,7 +1493,7 @@
       </c>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6">
       <c r="A60" s="2">
         <v>45622</v>
       </c>
@@ -1497,7 +1511,7 @@
       </c>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6">
       <c r="A61" s="2">
         <v>45622</v>
       </c>
@@ -1515,7 +1529,7 @@
       </c>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6">
       <c r="A62" s="2">
         <v>45623</v>
       </c>
@@ -1533,7 +1547,7 @@
       </c>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6">
       <c r="A63" s="2">
         <v>45623</v>
       </c>
@@ -1551,7 +1565,7 @@
       </c>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6">
       <c r="A64" s="2">
         <v>45629</v>
       </c>
@@ -1569,7 +1583,7 @@
       </c>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6">
       <c r="A65" s="2">
         <v>45629</v>
       </c>
@@ -1587,7 +1601,7 @@
       </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6">
       <c r="A66" s="2">
         <v>45635</v>
       </c>
@@ -1605,7 +1619,7 @@
       </c>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6">
       <c r="A67" s="2">
         <v>45635</v>
       </c>
@@ -1623,7 +1637,7 @@
       </c>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6">
       <c r="A68" s="2">
         <v>45636</v>
       </c>
@@ -1641,7 +1655,7 @@
       </c>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6">
       <c r="A69" s="2">
         <v>45637</v>
       </c>
@@ -1659,7 +1673,7 @@
       </c>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6">
       <c r="A70" s="2">
         <v>45637</v>
       </c>
@@ -1677,7 +1691,7 @@
       </c>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6">
       <c r="A71" s="2">
         <v>45638</v>
       </c>
@@ -1695,7 +1709,7 @@
       </c>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6">
       <c r="A72" s="2">
         <v>45638</v>
       </c>
@@ -1713,7 +1727,7 @@
       </c>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6">
       <c r="A73" s="2">
         <v>45640</v>
       </c>
@@ -1731,7 +1745,7 @@
       </c>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6">
       <c r="A74" s="2">
         <v>45640</v>
       </c>
@@ -1749,7 +1763,7 @@
       </c>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6">
       <c r="A75" s="2">
         <v>45640</v>
       </c>
@@ -1767,7 +1781,7 @@
       </c>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6">
       <c r="A76" s="2">
         <v>45659</v>
       </c>
@@ -1785,7 +1799,7 @@
       </c>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6">
       <c r="A77" s="2">
         <v>45659</v>
       </c>
@@ -1803,7 +1817,7 @@
       </c>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6">
       <c r="A78" s="2">
         <v>45659</v>
       </c>
@@ -1821,7 +1835,7 @@
       </c>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6">
       <c r="A79" s="2">
         <v>45660</v>
       </c>
@@ -1839,7 +1853,7 @@
       </c>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6">
       <c r="A80" s="2">
         <v>45660</v>
       </c>
@@ -1857,7 +1871,7 @@
       </c>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6">
       <c r="A81" s="2">
         <v>45661</v>
       </c>
@@ -1875,7 +1889,7 @@
       </c>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6">
       <c r="A82" s="2">
         <v>45661</v>
       </c>
@@ -1893,7 +1907,7 @@
       </c>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6">
       <c r="A83" s="2">
         <v>45661</v>
       </c>
@@ -1911,7 +1925,7 @@
       </c>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6">
       <c r="A84" s="2">
         <v>45662</v>
       </c>
@@ -1929,7 +1943,7 @@
       </c>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6">
       <c r="A85" s="2">
         <v>45662</v>
       </c>
@@ -1947,7 +1961,7 @@
       </c>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6">
       <c r="A86" s="2">
         <v>45663</v>
       </c>
@@ -1965,7 +1979,7 @@
       </c>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6">
       <c r="A87" s="2">
         <v>45663</v>
       </c>
@@ -1983,7 +1997,7 @@
       </c>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6">
       <c r="A88" s="2">
         <v>45663</v>
       </c>
@@ -2001,7 +2015,7 @@
       </c>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6">
       <c r="A89" s="2">
         <v>45670</v>
       </c>
@@ -2019,7 +2033,7 @@
       </c>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6">
       <c r="A90" s="2">
         <v>45670</v>
       </c>
@@ -2037,7 +2051,7 @@
       </c>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6">
       <c r="A91" s="2">
         <v>45670</v>
       </c>
@@ -2055,7 +2069,7 @@
       </c>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6">
       <c r="A92" s="2">
         <v>45677</v>
       </c>
@@ -2073,7 +2087,7 @@
       </c>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6">
       <c r="A93" s="2">
         <v>45677</v>
       </c>
@@ -2091,7 +2105,7 @@
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6">
       <c r="A94" s="2">
         <v>45677</v>
       </c>
@@ -2109,7 +2123,7 @@
       </c>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6">
       <c r="A95" s="2">
         <v>45678</v>
       </c>
@@ -2127,7 +2141,7 @@
       </c>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6">
       <c r="A96" s="2">
         <v>45678</v>
       </c>
@@ -2145,7 +2159,7 @@
       </c>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6">
       <c r="A97" s="2">
         <v>45678</v>
       </c>
@@ -2163,7 +2177,7 @@
       </c>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6">
       <c r="A98" s="2">
         <v>45678</v>
       </c>
@@ -2181,7 +2195,7 @@
       </c>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6">
       <c r="A99" s="2">
         <v>45680</v>
       </c>
@@ -2199,7 +2213,7 @@
       </c>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6">
       <c r="A100" s="2">
         <v>45680</v>
       </c>
@@ -2217,7 +2231,7 @@
       </c>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6">
       <c r="A101" s="2">
         <v>45680</v>
       </c>
@@ -2235,7 +2249,7 @@
       </c>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6">
       <c r="A102" s="2">
         <v>45681</v>
       </c>
@@ -2253,7 +2267,7 @@
       </c>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6">
       <c r="A103" s="2">
         <v>45681</v>
       </c>
@@ -2271,7 +2285,7 @@
       </c>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6">
       <c r="A104" s="2">
         <v>45681</v>
       </c>
@@ -2289,7 +2303,7 @@
       </c>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6">
       <c r="A105" s="2">
         <v>45681</v>
       </c>
@@ -2307,7 +2321,7 @@
       </c>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6">
       <c r="A106" s="2">
         <v>45682</v>
       </c>
@@ -2325,7 +2339,7 @@
       </c>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6">
       <c r="A107" s="2">
         <v>45682</v>
       </c>
@@ -2343,7 +2357,7 @@
       </c>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6">
       <c r="A108" s="2">
         <v>45682</v>
       </c>
@@ -2361,7 +2375,7 @@
       </c>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6">
       <c r="A109" s="2">
         <v>45682</v>
       </c>
@@ -2379,7 +2393,7 @@
       </c>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6">
       <c r="A110" s="2">
         <v>45682</v>
       </c>
@@ -2397,7 +2411,7 @@
       </c>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6">
       <c r="A111" s="2">
         <v>45683</v>
       </c>
@@ -2415,7 +2429,7 @@
       </c>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6">
       <c r="A112" s="2">
         <v>45683</v>
       </c>
@@ -2433,7 +2447,7 @@
       </c>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6">
       <c r="A113" s="2">
         <v>45683</v>
       </c>
@@ -2451,7 +2465,7 @@
       </c>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6">
       <c r="A114" s="2">
         <v>45683</v>
       </c>
@@ -2469,7 +2483,7 @@
       </c>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6">
       <c r="A115" s="2">
         <v>45684</v>
       </c>
@@ -2487,7 +2501,7 @@
       </c>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6">
       <c r="A116" s="2">
         <v>45684</v>
       </c>
@@ -2505,7 +2519,7 @@
       </c>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6">
       <c r="A117" s="2">
         <v>45684</v>
       </c>
@@ -2523,7 +2537,7 @@
       </c>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6">
       <c r="A118" s="2">
         <v>45685</v>
       </c>
@@ -2541,7 +2555,7 @@
       </c>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6">
       <c r="A119" s="2">
         <v>45686</v>
       </c>
@@ -2559,293 +2573,332 @@
       </c>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="1"/>
-      <c r="D120" s="1"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="1"/>
-      <c r="D121" s="1"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="1"/>
-      <c r="D122" s="1"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6">
+      <c r="A120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B120" t="s">
+        <v>11</v>
+      </c>
+      <c r="C120" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B121" t="s">
+        <v>13</v>
+      </c>
+      <c r="C121" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B122" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" s="1"/>
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6">
       <c r="A124" s="1"/>
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1">
       <c r="A147" s="1"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:1">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1">
       <c r="A200" s="1"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1">
       <c r="A202" s="1"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1">
       <c r="A203" s="1"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1">
       <c r="A204" s="1"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1">
       <c r="A205" s="1"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1">
       <c r="A206" s="1"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1">
       <c r="A207" s="1"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1">
       <c r="A208" s="1"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1">
       <c r="A209" s="1"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:1">
       <c r="A210" s="1"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:1">
       <c r="A211" s="1"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:1">
       <c r="A212" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+  <pageSetup horizontalDpi="180" r:id="rId1" orientation="portrait" paperSize="9" verticalDpi="180"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add 4 func to change task
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Number of task</t>
   </si>
@@ -36,31 +36,28 @@
     <t>0.3</t>
   </si>
   <si>
+    <t>скок решал</t>
+  </si>
+  <si>
     <t>0.2</t>
   </si>
   <si>
     <t>0.1</t>
   </si>
   <si>
-    <t>1</t>
+    <t>31-01-25</t>
   </si>
   <si>
-    <t>count solved</t>
+    <t>2</t>
   </si>
   <si>
-    <t>30-01-25</t>
+    <t>3</t>
   </si>
   <si>
-    <t>9999</t>
+    <t>4</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>9998</t>
-  </si>
-  <si>
-    <t>9997</t>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -97,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
@@ -107,9 +104,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F212"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -445,7 +439,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -456,7 +450,7 @@
       <c r="B2" s="1">
         <v>2239</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1">
@@ -474,7 +468,7 @@
       <c r="B3" s="1">
         <v>1768</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1">
@@ -486,20 +480,20 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2">
-        <v>45565</v>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>392</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -510,7 +504,7 @@
       <c r="B5" s="1">
         <v>121</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" s="1">
@@ -528,7 +522,7 @@
       <c r="B6" s="1">
         <v>13</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="1">
@@ -546,7 +540,7 @@
       <c r="B7" s="1">
         <v>217</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" s="1">
@@ -564,7 +558,7 @@
       <c r="B8" s="1">
         <v>242</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>0</v>
       </c>
       <c r="D8" s="1">
@@ -582,7 +576,7 @@
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="1">
         <v>0</v>
       </c>
       <c r="D9" s="1">
@@ -600,7 +594,7 @@
       <c r="B10" s="1">
         <v>49</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" s="1">
@@ -618,7 +612,7 @@
       <c r="B11" s="1">
         <v>238</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="1">
         <v>0</v>
       </c>
       <c r="D11" s="1">
@@ -636,7 +630,7 @@
       <c r="B12" s="1">
         <v>128</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>0</v>
       </c>
       <c r="D12" s="1">
@@ -654,7 +648,7 @@
       <c r="B13" s="1">
         <v>977</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="1">
         <v>0</v>
       </c>
       <c r="D13" s="1">
@@ -672,7 +666,7 @@
       <c r="B14" s="1">
         <v>14</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" s="1">
@@ -690,7 +684,7 @@
       <c r="B15" s="1">
         <v>125</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
@@ -708,7 +702,7 @@
       <c r="B16" s="1">
         <v>167</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" s="1">
@@ -726,7 +720,7 @@
       <c r="B17" s="1">
         <v>771</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" s="1">
@@ -744,7 +738,7 @@
       <c r="B18" s="1">
         <v>383</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18" s="1">
@@ -762,7 +756,7 @@
       <c r="B19" s="1">
         <v>1431</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" s="1">
@@ -780,7 +774,7 @@
       <c r="B20" s="1">
         <v>268</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="1">
         <v>0</v>
       </c>
       <c r="D20" s="1">
@@ -798,7 +792,7 @@
       <c r="B21" s="1">
         <v>75</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" s="1">
@@ -816,7 +810,7 @@
       <c r="B22" s="1">
         <v>2418</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="1">
@@ -834,7 +828,7 @@
       <c r="B23" s="1">
         <v>9</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23" s="1">
@@ -852,7 +846,7 @@
       <c r="B24" s="1">
         <v>389</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1">
@@ -870,7 +864,7 @@
       <c r="B25" s="1">
         <v>345</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="1">
         <v>0</v>
       </c>
       <c r="D25" s="1">
@@ -888,7 +882,7 @@
       <c r="B26" s="1">
         <v>151</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="1">
         <v>0</v>
       </c>
       <c r="D26" s="1">
@@ -906,7 +900,7 @@
       <c r="B27" s="1">
         <v>334</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1">
@@ -924,7 +918,7 @@
       <c r="B28" s="1">
         <v>27</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="1">
         <v>0</v>
       </c>
       <c r="D28" s="1">
@@ -942,7 +936,7 @@
       <c r="B29" s="1">
         <v>26</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="1">
         <v>0</v>
       </c>
       <c r="D29" s="1">
@@ -960,7 +954,7 @@
       <c r="B30" s="1">
         <v>80</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="1">
         <v>0</v>
       </c>
       <c r="D30" s="1">
@@ -978,7 +972,7 @@
       <c r="B31" s="1">
         <v>169</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="1">
         <v>0</v>
       </c>
       <c r="D31" s="1">
@@ -996,7 +990,7 @@
       <c r="B32" s="1">
         <v>88</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="1">
         <v>0</v>
       </c>
       <c r="D32" s="1">
@@ -1014,7 +1008,7 @@
       <c r="B33" s="1">
         <v>189</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1">
@@ -1032,7 +1026,7 @@
       <c r="B34" s="1">
         <v>58</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" s="1">
@@ -1050,7 +1044,7 @@
       <c r="B35" s="1">
         <v>443</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="1">
@@ -1068,7 +1062,7 @@
       <c r="B36" s="1">
         <v>283</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="1">
@@ -1081,13 +1075,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>45333</v>
+        <v>45598</v>
       </c>
       <c r="B37" s="1">
         <v>605</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>8</v>
+      <c r="C37" s="1">
+        <v>1</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
@@ -1104,7 +1098,7 @@
       <c r="B38" s="1">
         <v>643</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="1">
         <v>0</v>
       </c>
       <c r="D38" s="1">
@@ -1122,7 +1116,7 @@
       <c r="B39" s="1">
         <v>11</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" s="1">
@@ -1140,7 +1134,7 @@
       <c r="B40" s="1">
         <v>1679</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="1">
         <v>1</v>
       </c>
       <c r="D40" s="1">
@@ -1158,7 +1152,7 @@
       <c r="B41" s="1">
         <v>1732</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="1">
         <v>0</v>
       </c>
       <c r="D41" s="1">
@@ -1176,7 +1170,7 @@
       <c r="B42" s="1">
         <v>374</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="1">
@@ -1194,7 +1188,7 @@
       <c r="B43" s="1">
         <v>2300</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="1">
@@ -1212,7 +1206,7 @@
       <c r="B44" s="1">
         <v>338</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="1">
         <v>0</v>
       </c>
       <c r="D44" s="1">
@@ -1230,7 +1224,7 @@
       <c r="B45" s="1">
         <v>191</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="1">
         <v>0</v>
       </c>
       <c r="D45" s="1">
@@ -1248,7 +1242,7 @@
       <c r="B46" s="1">
         <v>136</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="1">
         <v>0</v>
       </c>
       <c r="D46" s="1">
@@ -1266,7 +1260,7 @@
       <c r="B47" s="1">
         <v>29</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="1">
         <v>0</v>
       </c>
       <c r="D47" s="1">
@@ -1284,7 +1278,7 @@
       <c r="B48" s="1">
         <v>202</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="1">
         <v>1</v>
       </c>
       <c r="D48" s="1">
@@ -1302,7 +1296,7 @@
       <c r="B49" s="1">
         <v>66</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="1">
         <v>0</v>
       </c>
       <c r="D49" s="1">
@@ -1314,20 +1308,20 @@
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="2">
-        <v>45618</v>
+      <c r="A50" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B50" s="1">
         <v>4</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="1">
         <v>3</v>
       </c>
-      <c r="E50" s="1">
-        <v>1</v>
+      <c r="E50" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F50" s="1"/>
     </row>
@@ -1338,7 +1332,7 @@
       <c r="B51" s="1">
         <v>1929</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="1">
         <v>0</v>
       </c>
       <c r="D51" s="1">
@@ -1356,7 +1350,7 @@
       <c r="B52" s="1">
         <v>1512</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="1">
         <v>0</v>
       </c>
       <c r="D52" s="1">
@@ -1374,7 +1368,7 @@
       <c r="B53" s="1">
         <v>3190</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="1">
         <v>0</v>
       </c>
       <c r="D53" s="1">
@@ -1392,7 +1386,7 @@
       <c r="B54" s="1">
         <v>3289</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="1">
         <v>0</v>
       </c>
       <c r="D54" s="1">
@@ -1410,7 +1404,7 @@
       <c r="B55" s="1">
         <v>34</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D55" s="1">
@@ -1428,7 +1422,7 @@
       <c r="B56" s="1">
         <v>2396</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1">
@@ -1446,7 +1440,7 @@
       <c r="B57" s="1">
         <v>2824</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="1">
         <v>0</v>
       </c>
       <c r="D57" s="1">
@@ -1459,19 +1453,19 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>45621</v>
+        <v>45687</v>
       </c>
       <c r="B58" s="1">
         <v>15</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58" s="1">
         <v>1</v>
       </c>
       <c r="D58" s="1">
         <v>2</v>
       </c>
       <c r="E58" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F58" s="1"/>
     </row>
@@ -1482,7 +1476,7 @@
       <c r="B59" s="1">
         <v>1108</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59" s="1">
         <v>0</v>
       </c>
       <c r="D59" s="1">
@@ -1500,7 +1494,7 @@
       <c r="B60" s="1">
         <v>206</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60" s="1">
         <v>1</v>
       </c>
       <c r="D60" s="1">
@@ -1518,7 +1512,7 @@
       <c r="B61" s="1">
         <v>2807</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61" s="1">
         <v>1</v>
       </c>
       <c r="D61" s="1">
@@ -1536,7 +1530,7 @@
       <c r="B62" s="1">
         <v>2181</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C62" s="1">
         <v>1</v>
       </c>
       <c r="D62" s="1">
@@ -1554,7 +1548,7 @@
       <c r="B63" s="1">
         <v>1290</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C63" s="1">
         <v>0</v>
       </c>
       <c r="D63" s="1">
@@ -1572,7 +1566,7 @@
       <c r="B64" s="1">
         <v>237</v>
       </c>
-      <c r="C64" s="4">
+      <c r="C64" s="1">
         <v>1</v>
       </c>
       <c r="D64" s="1">
@@ -1590,7 +1584,7 @@
       <c r="B65" s="1">
         <v>876</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65" s="1">
         <v>1</v>
       </c>
       <c r="D65" s="1">
@@ -1608,7 +1602,7 @@
       <c r="B66" s="1">
         <v>141</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="1">
@@ -1626,7 +1620,7 @@
       <c r="B67" s="1">
         <v>21</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67" s="1">
         <v>1</v>
       </c>
       <c r="D67" s="1">
@@ -1644,7 +1638,7 @@
       <c r="B68" s="1">
         <v>2095</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68" s="1">
         <v>1</v>
       </c>
       <c r="D68" s="1">
@@ -1662,7 +1656,7 @@
       <c r="B69" s="1">
         <v>2130</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C69" s="1">
         <v>1</v>
       </c>
       <c r="D69" s="1">
@@ -1680,7 +1674,7 @@
       <c r="B70" s="1">
         <v>234</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C70" s="1">
         <v>0</v>
       </c>
       <c r="D70" s="1">
@@ -1698,7 +1692,7 @@
       <c r="B71" s="1">
         <v>328</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D71" s="1">
@@ -1716,7 +1710,7 @@
       <c r="B72" s="1">
         <v>2558</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C72" s="1">
         <v>0</v>
       </c>
       <c r="D72" s="1">
@@ -1734,7 +1728,7 @@
       <c r="B73" s="1">
         <v>162</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="1">
         <v>1</v>
       </c>
       <c r="D73" s="1">
@@ -1752,7 +1746,7 @@
       <c r="B74" s="1">
         <v>2951</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74" s="1">
         <v>0</v>
       </c>
       <c r="D74" s="1">
@@ -1770,7 +1764,7 @@
       <c r="B75" s="1">
         <v>2210</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75" s="1">
         <v>1</v>
       </c>
       <c r="D75" s="1">
@@ -1788,7 +1782,7 @@
       <c r="B76" s="1">
         <v>2</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76" s="1">
         <v>1</v>
       </c>
       <c r="D76" s="1">
@@ -1806,7 +1800,7 @@
       <c r="B77" s="1">
         <v>67</v>
       </c>
-      <c r="C77" s="4">
+      <c r="C77" s="1">
         <v>1</v>
       </c>
       <c r="D77" s="1">
@@ -1824,7 +1818,7 @@
       <c r="B78" s="1">
         <v>43</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C78" s="1">
         <v>1</v>
       </c>
       <c r="D78" s="1">
@@ -1842,7 +1836,7 @@
       <c r="B79" s="1">
         <v>7</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C79" s="1">
         <v>0</v>
       </c>
       <c r="D79" s="1">
@@ -1860,7 +1854,7 @@
       <c r="B80" s="1">
         <v>190</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C80" s="1">
         <v>1</v>
       </c>
       <c r="D80" s="1">
@@ -1878,7 +1872,7 @@
       <c r="B81" s="1">
         <v>78</v>
       </c>
-      <c r="C81" s="4">
+      <c r="C81" s="1">
         <v>1</v>
       </c>
       <c r="D81" s="1">
@@ -1896,7 +1890,7 @@
       <c r="B82" s="1">
         <v>118</v>
       </c>
-      <c r="C82" s="4">
+      <c r="C82" s="1">
         <v>0</v>
       </c>
       <c r="D82" s="1">
@@ -1914,7 +1908,7 @@
       <c r="B83" s="1">
         <v>119</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C83" s="1">
         <v>0</v>
       </c>
       <c r="D83" s="1">
@@ -1932,7 +1926,7 @@
       <c r="B84" s="1">
         <v>33</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C84" s="1">
         <v>1</v>
       </c>
       <c r="D84" s="1">
@@ -1950,7 +1944,7 @@
       <c r="B85" s="1">
         <v>2381</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85" s="1">
         <v>2</v>
       </c>
       <c r="D85" s="1">
@@ -1968,7 +1962,7 @@
       <c r="B86" s="1">
         <v>104</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86" s="1">
         <v>1</v>
       </c>
       <c r="D86" s="1">
@@ -1986,7 +1980,7 @@
       <c r="B87" s="1">
         <v>94</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C87" s="1">
         <v>1</v>
       </c>
       <c r="D87" s="1">
@@ -2004,7 +1998,7 @@
       <c r="B88" s="1">
         <v>20</v>
       </c>
-      <c r="C88" s="4">
+      <c r="C88" s="1">
         <v>1</v>
       </c>
       <c r="D88" s="1">
@@ -2022,7 +2016,7 @@
       <c r="B89" s="1">
         <v>287</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C89" s="1">
         <v>1</v>
       </c>
       <c r="D89" s="1">
@@ -2040,7 +2034,7 @@
       <c r="B90" s="1">
         <v>645</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D90" s="1">
@@ -2058,7 +2052,7 @@
       <c r="B91" s="1">
         <v>41</v>
       </c>
-      <c r="C91" s="4">
+      <c r="C91" s="1">
         <v>0</v>
       </c>
       <c r="D91" s="1">
@@ -2076,7 +2070,7 @@
       <c r="B92" s="1">
         <v>1816</v>
       </c>
-      <c r="C92" s="4">
+      <c r="C92" s="1">
         <v>0</v>
       </c>
       <c r="D92" s="1">
@@ -2094,7 +2088,7 @@
       <c r="B93" s="1">
         <v>1572</v>
       </c>
-      <c r="C93" s="4">
+      <c r="C93" s="1">
         <v>0</v>
       </c>
       <c r="D93" s="1">
@@ -2112,7 +2106,7 @@
       <c r="B94" s="1">
         <v>2319</v>
       </c>
-      <c r="C94" s="4">
+      <c r="C94" s="1">
         <v>0</v>
       </c>
       <c r="D94" s="1">
@@ -2130,7 +2124,7 @@
       <c r="B95" s="1">
         <v>278</v>
       </c>
-      <c r="C95" s="4">
+      <c r="C95" s="1">
         <v>1</v>
       </c>
       <c r="D95" s="1">
@@ -2148,7 +2142,7 @@
       <c r="B96" s="1">
         <v>2089</v>
       </c>
-      <c r="C96" s="4">
+      <c r="C96" s="1">
         <v>0</v>
       </c>
       <c r="D96" s="1">
@@ -2166,7 +2160,7 @@
       <c r="B97" s="1">
         <v>744</v>
       </c>
-      <c r="C97" s="4">
+      <c r="C97" s="1">
         <v>1</v>
       </c>
       <c r="D97" s="1">
@@ -2184,7 +2178,7 @@
       <c r="B98" s="1">
         <v>441</v>
       </c>
-      <c r="C98" s="4">
+      <c r="C98" s="1">
         <v>0</v>
       </c>
       <c r="D98" s="1">
@@ -2202,7 +2196,7 @@
       <c r="B99" s="1">
         <v>349</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="1">
@@ -2220,7 +2214,7 @@
       <c r="B100" s="1">
         <v>350</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="1">
@@ -2238,7 +2232,7 @@
       <c r="B101" s="1">
         <v>2529</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="C101" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D101" s="1">
@@ -2256,7 +2250,7 @@
       <c r="B102" s="1">
         <v>448</v>
       </c>
-      <c r="C102" s="4">
+      <c r="C102" s="1">
         <v>0</v>
       </c>
       <c r="D102" s="1">
@@ -2274,7 +2268,7 @@
       <c r="B103" s="1">
         <v>442</v>
       </c>
-      <c r="C103" s="4">
+      <c r="C103" s="1">
         <v>0</v>
       </c>
       <c r="D103" s="1">
@@ -2292,7 +2286,7 @@
       <c r="B104" s="1">
         <v>70</v>
       </c>
-      <c r="C104" s="4">
+      <c r="C104" s="1">
         <v>1</v>
       </c>
       <c r="D104" s="1">
@@ -2310,7 +2304,7 @@
       <c r="B105" s="1">
         <v>1351</v>
       </c>
-      <c r="C105" s="4">
+      <c r="C105" s="1">
         <v>0</v>
       </c>
       <c r="D105" s="1">
@@ -2328,7 +2322,7 @@
       <c r="B106" s="1">
         <v>89</v>
       </c>
-      <c r="C106" s="4">
+      <c r="C106" s="1">
         <v>1</v>
       </c>
       <c r="D106" s="1">
@@ -2346,7 +2340,7 @@
       <c r="B107" s="1">
         <v>1071</v>
       </c>
-      <c r="C107" s="4">
+      <c r="C107" s="1">
         <v>1</v>
       </c>
       <c r="D107" s="1">
@@ -2364,7 +2358,7 @@
       <c r="B108" s="1">
         <v>1979</v>
       </c>
-      <c r="C108" s="4">
+      <c r="C108" s="1">
         <v>0</v>
       </c>
       <c r="D108" s="1">
@@ -2382,7 +2376,7 @@
       <c r="B109" s="1">
         <v>1952</v>
       </c>
-      <c r="C109" s="4">
+      <c r="C109" s="1">
         <v>0</v>
       </c>
       <c r="D109" s="1">
@@ -2400,7 +2394,7 @@
       <c r="B110" s="1">
         <v>2413</v>
       </c>
-      <c r="C110" s="4">
+      <c r="C110" s="1">
         <v>0</v>
       </c>
       <c r="D110" s="1">
@@ -2418,7 +2412,7 @@
       <c r="B111" s="1">
         <v>137</v>
       </c>
-      <c r="C111" s="4">
+      <c r="C111" s="1">
         <v>0</v>
       </c>
       <c r="D111" s="1">
@@ -2436,7 +2430,7 @@
       <c r="B112" s="1">
         <v>260</v>
       </c>
-      <c r="C112" s="4">
+      <c r="C112" s="1">
         <v>0</v>
       </c>
       <c r="D112" s="1">
@@ -2454,8 +2448,8 @@
       <c r="B113" s="1">
         <v>3158</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>6</v>
+      <c r="C113" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D113" s="1">
         <v>1</v>
@@ -2472,8 +2466,8 @@
       <c r="B114" s="1">
         <v>3162</v>
       </c>
-      <c r="C114" s="4" t="s">
-        <v>6</v>
+      <c r="C114" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D114" s="1">
         <v>1</v>
@@ -2490,7 +2484,7 @@
       <c r="B115" s="1">
         <v>74</v>
       </c>
-      <c r="C115" s="4">
+      <c r="C115" s="1">
         <v>0</v>
       </c>
       <c r="D115" s="1">
@@ -2508,7 +2502,7 @@
       <c r="B116" s="1">
         <v>153</v>
       </c>
-      <c r="C116" s="4">
+      <c r="C116" s="1">
         <v>0</v>
       </c>
       <c r="D116" s="1">
@@ -2526,7 +2520,7 @@
       <c r="B117" s="1">
         <v>240</v>
       </c>
-      <c r="C117" s="4">
+      <c r="C117" s="1">
         <v>0</v>
       </c>
       <c r="D117" s="1">
@@ -2544,8 +2538,8 @@
       <c r="B118" s="1">
         <v>347</v>
       </c>
-      <c r="C118" s="4" t="s">
-        <v>6</v>
+      <c r="C118" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D118" s="1">
         <v>2</v>
@@ -2562,8 +2556,8 @@
       <c r="B119" s="1">
         <v>680</v>
       </c>
-      <c r="C119" s="4" t="s">
-        <v>7</v>
+      <c r="C119" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
@@ -2574,55 +2568,29 @@
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B120" t="s">
-        <v>11</v>
-      </c>
-      <c r="C120" t="s">
-        <v>12</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E120" t="s">
-        <v>8</v>
+      <c r="A120" s="2">
+        <v>45687</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2443</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0</v>
+      </c>
+      <c r="D120" s="1">
+        <v>2</v>
+      </c>
+      <c r="E120" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B121" t="s">
-        <v>13</v>
-      </c>
-      <c r="C121" t="s">
-        <v>12</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E121" t="s">
-        <v>8</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="D121" s="1"/>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B122" t="s">
-        <v>14</v>
-      </c>
-      <c r="C122" t="s">
-        <v>12</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E122" t="s">
-        <v>8</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="D122" s="1"/>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="1"/>

</xml_diff>

<commit_message>
change logic of work tasks
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Number of task</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9998</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -493,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2585,8 +2600,21 @@
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="1"/>
-      <c r="D121" s="1"/>
+      <c r="A121" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" t="s">
+        <v>16</v>
+      </c>
+      <c r="C121" t="s">
+        <v>17</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E121" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="1"/>

</xml_diff>

<commit_message>
rechange project + add postgree db
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="263">
   <si>
     <t>Number of task</t>
   </si>
@@ -178,6 +178,633 @@
   </si>
   <si>
     <t>3160</t>
+  </si>
+  <si>
+    <t>08-02-25</t>
+  </si>
+  <si>
+    <t>2349</t>
+  </si>
+  <si>
+    <t>10-02-25</t>
+  </si>
+  <si>
+    <t>498</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>11-02-25</t>
+  </si>
+  <si>
+    <t>1910</t>
+  </si>
+  <si>
+    <t>557</t>
+  </si>
+  <si>
+    <t>14-02-25</t>
+  </si>
+  <si>
+    <t>1352</t>
+  </si>
+  <si>
+    <t>707</t>
+  </si>
+  <si>
+    <t>16-02-25</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>17-02-25</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>18-02-25</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>912</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>19-02-25</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>2390</t>
+  </si>
+  <si>
+    <t>735</t>
+  </si>
+  <si>
+    <t>20-02-25</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1464</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>21-02-25</t>
+  </si>
+  <si>
+    <t>2415</t>
+  </si>
+  <si>
+    <t>938</t>
+  </si>
+  <si>
+    <t>1302</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>22-02-25</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>3340</t>
+  </si>
+  <si>
+    <t>23-02-25</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>1161</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>24-02-25</t>
+  </si>
+  <si>
+    <t>2215</t>
+  </si>
+  <si>
+    <t>637</t>
+  </si>
+  <si>
+    <t>25-02-25</t>
+  </si>
+  <si>
+    <t>709</t>
+  </si>
+  <si>
+    <t>2894</t>
+  </si>
+  <si>
+    <t>2129</t>
+  </si>
+  <si>
+    <t>3120</t>
+  </si>
+  <si>
+    <t>2309</t>
+  </si>
+  <si>
+    <t>26-02-25</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
+    <t>2544</t>
+  </si>
+  <si>
+    <t>2553</t>
+  </si>
+  <si>
+    <t>27-02-25</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>28-02-25</t>
+  </si>
+  <si>
+    <t>2798</t>
+  </si>
+  <si>
+    <t>3065</t>
+  </si>
+  <si>
+    <t>1389</t>
+  </si>
+  <si>
+    <t>01-03-25</t>
+  </si>
+  <si>
+    <t>2460</t>
+  </si>
+  <si>
+    <t>513</t>
+  </si>
+  <si>
+    <t>896</t>
+  </si>
+  <si>
+    <t>1822</t>
+  </si>
+  <si>
+    <t>02-03-25</t>
+  </si>
+  <si>
+    <t>2570</t>
+  </si>
+  <si>
+    <t>2363</t>
+  </si>
+  <si>
+    <t>1502</t>
+  </si>
+  <si>
+    <t>1523</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>03-03-25</t>
+  </si>
+  <si>
+    <t>2161</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>476</t>
+  </si>
+  <si>
+    <t>04-03-25</t>
+  </si>
+  <si>
+    <t>965</t>
+  </si>
+  <si>
+    <t>326</t>
+  </si>
+  <si>
+    <t>1009</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>342</t>
+  </si>
+  <si>
+    <t>3280</t>
+  </si>
+  <si>
+    <t>05-03-25</t>
+  </si>
+  <si>
+    <t>2579</t>
+  </si>
+  <si>
+    <t>06-03-25</t>
+  </si>
+  <si>
+    <t>867</t>
+  </si>
+  <si>
+    <t>3005</t>
+  </si>
+  <si>
+    <t>2965</t>
+  </si>
+  <si>
+    <t>3467</t>
+  </si>
+  <si>
+    <t>07-03-25</t>
+  </si>
+  <si>
+    <t>2523</t>
+  </si>
+  <si>
+    <t>1493</t>
+  </si>
+  <si>
+    <t>1748</t>
+  </si>
+  <si>
+    <t>451</t>
+  </si>
+  <si>
+    <t>08-03-25</t>
+  </si>
+  <si>
+    <t>3264</t>
+  </si>
+  <si>
+    <t>2974</t>
+  </si>
+  <si>
+    <t>2379</t>
+  </si>
+  <si>
+    <t>10-03-25</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>2357</t>
+  </si>
+  <si>
+    <t>3306</t>
+  </si>
+  <si>
+    <t>506</t>
+  </si>
+  <si>
+    <t>11-03-25</t>
+  </si>
+  <si>
+    <t>1365</t>
+  </si>
+  <si>
+    <t>2956</t>
+  </si>
+  <si>
+    <t>1038</t>
+  </si>
+  <si>
+    <t>796</t>
+  </si>
+  <si>
+    <t>1358</t>
+  </si>
+  <si>
+    <t>12-03-25</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>13-03-25</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>2265</t>
+  </si>
+  <si>
+    <t>3356</t>
+  </si>
+  <si>
+    <t>14-03-25</t>
+  </si>
+  <si>
+    <t>530</t>
+  </si>
+  <si>
+    <t>15-03-25</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>1221</t>
+  </si>
+  <si>
+    <t>2788</t>
+  </si>
+  <si>
+    <t>2560</t>
+  </si>
+  <si>
+    <t>16-03-25</t>
+  </si>
+  <si>
+    <t>2594</t>
+  </si>
+  <si>
+    <t>17-03-25</t>
+  </si>
+  <si>
+    <t>2206</t>
+  </si>
+  <si>
+    <t>1832</t>
+  </si>
+  <si>
+    <t>2610</t>
+  </si>
+  <si>
+    <t>18-03-25</t>
+  </si>
+  <si>
+    <t>2401</t>
+  </si>
+  <si>
+    <t>19-03-25</t>
+  </si>
+  <si>
+    <t>3191</t>
+  </si>
+  <si>
+    <t>1684</t>
+  </si>
+  <si>
+    <t>20-03-25</t>
+  </si>
+  <si>
+    <t>3108</t>
+  </si>
+  <si>
+    <t>2236</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>21-03-25</t>
+  </si>
+  <si>
+    <t>875</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>2133</t>
+  </si>
+  <si>
+    <t>22-03-25</t>
+  </si>
+  <si>
+    <t>1669</t>
+  </si>
+  <si>
+    <t>1019</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>23-03-25</t>
+  </si>
+  <si>
+    <t>274</t>
+  </si>
+  <si>
+    <t>24-03-25</t>
+  </si>
+  <si>
+    <t>2785</t>
+  </si>
+  <si>
+    <t>2441</t>
+  </si>
+  <si>
+    <t>25-03-25</t>
+  </si>
+  <si>
+    <t>872</t>
+  </si>
+  <si>
+    <t>1448</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>26-03-25</t>
+  </si>
+  <si>
+    <t>2033</t>
+  </si>
+  <si>
+    <t>462</t>
+  </si>
+  <si>
+    <t>3146</t>
+  </si>
+  <si>
+    <t>1678</t>
+  </si>
+  <si>
+    <t>27-03-25</t>
+  </si>
+  <si>
+    <t>1315</t>
+  </si>
+  <si>
+    <t>739</t>
+  </si>
+  <si>
+    <t>28-03-25</t>
+  </si>
+  <si>
+    <t>30-03-25</t>
+  </si>
+  <si>
+    <t>2044</t>
+  </si>
+  <si>
+    <t>03-04-25</t>
+  </si>
+  <si>
+    <t>2367</t>
+  </si>
+  <si>
+    <t>2475</t>
+  </si>
+  <si>
+    <t>2465</t>
+  </si>
+  <si>
+    <t>04-04-25</t>
+  </si>
+  <si>
+    <t>1123</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>05-04-25</t>
+  </si>
+  <si>
+    <t>437</t>
+  </si>
+  <si>
+    <t>07-04-25</t>
+  </si>
+  <si>
+    <t>2114</t>
+  </si>
+  <si>
+    <t>2047</t>
+  </si>
+  <si>
+    <t>14-04-25</t>
+  </si>
+  <si>
+    <t>1534</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>15-04-25</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>2517</t>
+  </si>
+  <si>
+    <t>17-04-25</t>
+  </si>
+  <si>
+    <t>2176</t>
+  </si>
+  <si>
+    <t>18-04-25</t>
+  </si>
+  <si>
+    <t>2545</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>22-04-25</t>
+  </si>
+  <si>
+    <t>3512</t>
+  </si>
+  <si>
+    <t>2160</t>
+  </si>
+  <si>
+    <t>2535</t>
+  </si>
+  <si>
+    <t>23-04-25</t>
+  </si>
+  <si>
+    <t>1399</t>
+  </si>
+  <si>
+    <t>543</t>
   </si>
 </sst>
 </file>
@@ -783,20 +1410,20 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="2">
-        <v>45569</v>
+      <c r="A14" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="B14" s="1">
         <v>14</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="1">
-        <v>1</v>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -909,8 +1536,8 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2">
-        <v>45582</v>
+      <c r="A21" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B21" s="1">
         <v>75</v>
@@ -921,8 +1548,8 @@
       <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="E21" s="1">
-        <v>1</v>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -1233,8 +1860,8 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="2">
-        <v>45604</v>
+      <c r="A39" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B39" s="1">
         <v>11</v>
@@ -1245,8 +1872,8 @@
       <c r="D39" s="1">
         <v>2</v>
       </c>
-      <c r="E39" s="1">
-        <v>1</v>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -1287,20 +1914,20 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="2">
-        <v>45610</v>
+      <c r="A42" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="B42" s="1">
         <v>374</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
       </c>
-      <c r="E42" s="1">
-        <v>1</v>
+      <c r="E42" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="F42" s="1"/>
     </row>
@@ -1611,8 +2238,8 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="2">
-        <v>45622</v>
+      <c r="A60" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B60" s="1">
         <v>206</v>
@@ -1623,8 +2250,8 @@
       <c r="D60" s="1">
         <v>1</v>
       </c>
-      <c r="E60" s="1">
-        <v>1</v>
+      <c r="E60" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F60" s="1"/>
     </row>
@@ -1683,8 +2310,8 @@
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="2">
-        <v>45629</v>
+      <c r="A64" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B64" s="1">
         <v>237</v>
@@ -1695,8 +2322,8 @@
       <c r="D64" s="1">
         <v>2</v>
       </c>
-      <c r="E64" s="1">
-        <v>1</v>
+      <c r="E64" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F64" s="1"/>
     </row>
@@ -1737,20 +2364,20 @@
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="2">
-        <v>45635</v>
+      <c r="A67" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="B67" s="1">
         <v>21</v>
       </c>
-      <c r="C67" s="1">
-        <v>1</v>
+      <c r="C67" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D67" s="1">
         <v>2</v>
       </c>
-      <c r="E67" s="1">
-        <v>1</v>
+      <c r="E67" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F67" s="1"/>
     </row>
@@ -1773,20 +2400,20 @@
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="2">
-        <v>45637</v>
+      <c r="A69" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="B69" s="1">
         <v>2130</v>
       </c>
-      <c r="C69" s="1">
-        <v>1</v>
+      <c r="C69" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D69" s="1">
         <v>2</v>
       </c>
-      <c r="E69" s="1">
-        <v>1</v>
+      <c r="E69" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F69" s="1"/>
     </row>
@@ -1899,8 +2526,8 @@
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="2">
-        <v>45659</v>
+      <c r="A76" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="B76" s="1">
         <v>2</v>
@@ -1911,14 +2538,14 @@
       <c r="D76" s="1">
         <v>2</v>
       </c>
-      <c r="E76" s="1">
-        <v>1</v>
+      <c r="E76" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="2">
-        <v>45659</v>
+      <c r="A77" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B77" s="1">
         <v>67</v>
@@ -1929,8 +2556,8 @@
       <c r="D77" s="1">
         <v>1</v>
       </c>
-      <c r="E77" s="1">
-        <v>1</v>
+      <c r="E77" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F77" s="1"/>
     </row>
@@ -2007,8 +2634,8 @@
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="2">
-        <v>45661</v>
+      <c r="A82" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B82" s="1">
         <v>118</v>
@@ -2019,8 +2646,8 @@
       <c r="D82" s="1">
         <v>1</v>
       </c>
-      <c r="E82" s="1">
-        <v>1</v>
+      <c r="E82" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F82" s="1"/>
     </row>
@@ -2079,8 +2706,8 @@
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="2">
-        <v>45663</v>
+      <c r="A86" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B86" s="1">
         <v>104</v>
@@ -2091,8 +2718,8 @@
       <c r="D86" s="1">
         <v>1</v>
       </c>
-      <c r="E86" s="1">
-        <v>1</v>
+      <c r="E86" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F86" s="1"/>
     </row>
@@ -2115,8 +2742,8 @@
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="2">
-        <v>45663</v>
+      <c r="A88" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B88" s="1">
         <v>20</v>
@@ -2127,8 +2754,8 @@
       <c r="D88" s="1">
         <v>1</v>
       </c>
-      <c r="E88" s="1">
-        <v>1</v>
+      <c r="E88" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F88" s="1"/>
     </row>
@@ -2278,19 +2905,19 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2" t="s">
-        <v>46</v>
+        <v>183</v>
       </c>
       <c r="B97" s="1">
         <v>744</v>
       </c>
-      <c r="C97" s="1">
-        <v>1</v>
+      <c r="C97" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D97" s="1">
         <v>1</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="F97" s="1"/>
     </row>
@@ -2349,20 +2976,20 @@
       <c r="F100" s="1"/>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="2">
-        <v>45680</v>
+      <c r="A101" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="B101" s="1">
         <v>2529</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
-      <c r="E101" s="1">
-        <v>1</v>
+      <c r="E101" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="F101" s="1"/>
     </row>
@@ -3236,7 +3863,7 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B152" t="s">
         <v>51</v>
@@ -3248,12 +3875,12 @@
         <v>12</v>
       </c>
       <c r="E152" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B153" t="s">
         <v>52</v>
@@ -3265,7 +3892,7 @@
         <v>13</v>
       </c>
       <c r="E153" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -3286,178 +3913,2588 @@
       </c>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155" s="1"/>
+      <c r="A155" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B155" t="s">
+        <v>55</v>
+      </c>
+      <c r="C155" t="s">
+        <v>12</v>
+      </c>
+      <c r="D155" t="s">
+        <v>13</v>
+      </c>
+      <c r="E155" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="156" spans="1:3">
-      <c r="A156" s="1"/>
+      <c r="A156" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B156" t="s">
+        <v>57</v>
+      </c>
+      <c r="C156" t="s">
+        <v>12</v>
+      </c>
+      <c r="D156" t="s">
+        <v>13</v>
+      </c>
+      <c r="E156" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="1"/>
+      <c r="A157" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B157" t="s">
+        <v>58</v>
+      </c>
+      <c r="C157" t="s">
+        <v>12</v>
+      </c>
+      <c r="D157" t="s">
+        <v>13</v>
+      </c>
+      <c r="E157" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="1"/>
+      <c r="A158" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B158" t="s">
+        <v>60</v>
+      </c>
+      <c r="C158" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" t="s">
+        <v>13</v>
+      </c>
+      <c r="E158" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="159" spans="1:3">
-      <c r="A159" s="1"/>
+      <c r="A159" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B159" t="s">
+        <v>61</v>
+      </c>
+      <c r="C159" t="s">
+        <v>11</v>
+      </c>
+      <c r="D159" t="s">
+        <v>12</v>
+      </c>
+      <c r="E159" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" s="1"/>
+      <c r="A160" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B160" t="s">
+        <v>63</v>
+      </c>
+      <c r="C160" t="s">
+        <v>12</v>
+      </c>
+      <c r="D160" t="s">
+        <v>13</v>
+      </c>
+      <c r="E160" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="1"/>
+      <c r="A161" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B161" t="s">
+        <v>64</v>
+      </c>
+      <c r="C161" t="s">
+        <v>12</v>
+      </c>
+      <c r="D161" t="s">
+        <v>13</v>
+      </c>
+      <c r="E161" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="1"/>
+      <c r="A162" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B162" t="s">
+        <v>66</v>
+      </c>
+      <c r="C162" t="s">
+        <v>11</v>
+      </c>
+      <c r="D162" t="s">
+        <v>67</v>
+      </c>
+      <c r="E162" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="163" spans="1:1">
-      <c r="A163" s="1"/>
+      <c r="A163" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B163" t="s">
+        <v>68</v>
+      </c>
+      <c r="C163" t="s">
+        <v>11</v>
+      </c>
+      <c r="D163" t="s">
+        <v>13</v>
+      </c>
+      <c r="E163" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="1"/>
+      <c r="A164" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B164" t="s">
+        <v>69</v>
+      </c>
+      <c r="C164" t="s">
+        <v>11</v>
+      </c>
+      <c r="D164" t="s">
+        <v>13</v>
+      </c>
+      <c r="E164" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="1"/>
+      <c r="A165" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B165" t="s">
+        <v>71</v>
+      </c>
+      <c r="C165" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" t="s">
+        <v>12</v>
+      </c>
+      <c r="E165" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="1"/>
+      <c r="A166" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B166" t="s">
+        <v>72</v>
+      </c>
+      <c r="C166" t="s">
+        <v>12</v>
+      </c>
+      <c r="D166" t="s">
+        <v>12</v>
+      </c>
+      <c r="E166" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="1"/>
+      <c r="A167" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B167" t="s">
+        <v>74</v>
+      </c>
+      <c r="C167" t="s">
+        <v>11</v>
+      </c>
+      <c r="D167" t="s">
+        <v>13</v>
+      </c>
+      <c r="E167" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="1"/>
+      <c r="A168" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B168" t="s">
+        <v>75</v>
+      </c>
+      <c r="C168" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" t="s">
+        <v>13</v>
+      </c>
+      <c r="E168" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="1"/>
+      <c r="A169" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B169" t="s">
+        <v>76</v>
+      </c>
+      <c r="C169" t="s">
+        <v>11</v>
+      </c>
+      <c r="D169" t="s">
+        <v>13</v>
+      </c>
+      <c r="E169" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="1"/>
+      <c r="A170" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B170" t="s">
+        <v>77</v>
+      </c>
+      <c r="C170" t="s">
+        <v>11</v>
+      </c>
+      <c r="D170" t="s">
+        <v>12</v>
+      </c>
+      <c r="E170" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="1"/>
+      <c r="A171" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B171" t="s">
+        <v>79</v>
+      </c>
+      <c r="C171" t="s">
+        <v>11</v>
+      </c>
+      <c r="D171" t="s">
+        <v>12</v>
+      </c>
+      <c r="E171" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="1"/>
+      <c r="A172" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B172" t="s">
+        <v>80</v>
+      </c>
+      <c r="C172" t="s">
+        <v>11</v>
+      </c>
+      <c r="D172" t="s">
+        <v>12</v>
+      </c>
+      <c r="E172" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173" s="1"/>
+      <c r="A173" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B173" t="s">
+        <v>81</v>
+      </c>
+      <c r="C173" t="s">
+        <v>12</v>
+      </c>
+      <c r="D173" t="s">
+        <v>13</v>
+      </c>
+      <c r="E173" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="1"/>
+      <c r="A174" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B174" t="s">
+        <v>82</v>
+      </c>
+      <c r="C174" t="s">
+        <v>11</v>
+      </c>
+      <c r="D174" t="s">
+        <v>13</v>
+      </c>
+      <c r="E174" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="175" spans="1:1">
-      <c r="A175" s="1"/>
+      <c r="A175" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B175" t="s">
+        <v>83</v>
+      </c>
+      <c r="C175" t="s">
+        <v>11</v>
+      </c>
+      <c r="D175" t="s">
+        <v>13</v>
+      </c>
+      <c r="E175" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="1"/>
+      <c r="A176" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B176" t="s">
+        <v>84</v>
+      </c>
+      <c r="C176" t="s">
+        <v>12</v>
+      </c>
+      <c r="D176" t="s">
+        <v>13</v>
+      </c>
+      <c r="E176" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="177" spans="1:1">
-      <c r="A177" s="1"/>
+      <c r="A177" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B177" t="s">
+        <v>86</v>
+      </c>
+      <c r="C177" t="s">
+        <v>12</v>
+      </c>
+      <c r="D177" t="s">
+        <v>13</v>
+      </c>
+      <c r="E177" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178" s="1"/>
+      <c r="A178" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B178" t="s">
+        <v>87</v>
+      </c>
+      <c r="C178" t="s">
+        <v>11</v>
+      </c>
+      <c r="D178" t="s">
+        <v>12</v>
+      </c>
+      <c r="E178" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="179" spans="1:1">
-      <c r="A179" s="1"/>
+      <c r="A179" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B179" t="s">
+        <v>67</v>
+      </c>
+      <c r="C179" t="s">
+        <v>12</v>
+      </c>
+      <c r="D179" t="s">
+        <v>13</v>
+      </c>
+      <c r="E179" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="180" spans="1:1">
-      <c r="A180" s="1"/>
+      <c r="A180" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B180" t="s">
+        <v>88</v>
+      </c>
+      <c r="C180" t="s">
+        <v>12</v>
+      </c>
+      <c r="D180" t="s">
+        <v>12</v>
+      </c>
+      <c r="E180" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="181" spans="1:1">
-      <c r="A181" s="1"/>
+      <c r="A181" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B181" t="s">
+        <v>90</v>
+      </c>
+      <c r="C181" t="s">
+        <v>12</v>
+      </c>
+      <c r="D181" t="s">
+        <v>13</v>
+      </c>
+      <c r="E181" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="182" spans="1:1">
-      <c r="A182" s="1"/>
+      <c r="A182" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B182" t="s">
+        <v>91</v>
+      </c>
+      <c r="C182" t="s">
+        <v>12</v>
+      </c>
+      <c r="D182" t="s">
+        <v>12</v>
+      </c>
+      <c r="E182" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="183" spans="1:1">
-      <c r="A183" s="1"/>
+      <c r="A183" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B183" t="s">
+        <v>92</v>
+      </c>
+      <c r="C183" t="s">
+        <v>11</v>
+      </c>
+      <c r="D183" t="s">
+        <v>13</v>
+      </c>
+      <c r="E183" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="184" spans="1:1">
-      <c r="A184" s="1"/>
+      <c r="A184" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B184" t="s">
+        <v>93</v>
+      </c>
+      <c r="C184" t="s">
+        <v>11</v>
+      </c>
+      <c r="D184" t="s">
+        <v>12</v>
+      </c>
+      <c r="E184" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="185" spans="1:1">
-      <c r="A185" s="1"/>
+      <c r="A185" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B185" t="s">
+        <v>95</v>
+      </c>
+      <c r="C185" t="s">
+        <v>12</v>
+      </c>
+      <c r="D185" t="s">
+        <v>12</v>
+      </c>
+      <c r="E185" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" s="1"/>
+      <c r="A186" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B186" t="s">
+        <v>96</v>
+      </c>
+      <c r="C186" t="s">
+        <v>11</v>
+      </c>
+      <c r="D186" t="s">
+        <v>12</v>
+      </c>
+      <c r="E186" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="187" spans="1:1">
-      <c r="A187" s="1"/>
+      <c r="A187" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B187" t="s">
+        <v>97</v>
+      </c>
+      <c r="C187" t="s">
+        <v>11</v>
+      </c>
+      <c r="D187" t="s">
+        <v>13</v>
+      </c>
+      <c r="E187" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188" s="1"/>
+      <c r="A188" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B188" t="s">
+        <v>98</v>
+      </c>
+      <c r="C188" t="s">
+        <v>11</v>
+      </c>
+      <c r="D188" t="s">
+        <v>13</v>
+      </c>
+      <c r="E188" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="189" spans="1:1">
-      <c r="A189" s="1"/>
+      <c r="A189" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B189" t="s">
+        <v>99</v>
+      </c>
+      <c r="C189" t="s">
+        <v>11</v>
+      </c>
+      <c r="D189" t="s">
+        <v>12</v>
+      </c>
+      <c r="E189" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="190" spans="1:1">
-      <c r="A190" s="1"/>
+      <c r="A190" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B190" t="s">
+        <v>100</v>
+      </c>
+      <c r="C190" t="s">
+        <v>11</v>
+      </c>
+      <c r="D190" t="s">
+        <v>12</v>
+      </c>
+      <c r="E190" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="191" spans="1:1">
-      <c r="A191" s="1"/>
+      <c r="A191" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B191" t="s">
+        <v>102</v>
+      </c>
+      <c r="C191" t="s">
+        <v>11</v>
+      </c>
+      <c r="D191" t="s">
+        <v>13</v>
+      </c>
+      <c r="E191" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="192" spans="1:1">
-      <c r="A192" s="1"/>
+      <c r="A192" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B192" t="s">
+        <v>103</v>
+      </c>
+      <c r="C192" t="s">
+        <v>11</v>
+      </c>
+      <c r="D192" t="s">
+        <v>13</v>
+      </c>
+      <c r="E192" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="193" spans="1:1">
-      <c r="A193" s="1"/>
+      <c r="A193" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B193" t="s">
+        <v>104</v>
+      </c>
+      <c r="C193" t="s">
+        <v>11</v>
+      </c>
+      <c r="D193" t="s">
+        <v>13</v>
+      </c>
+      <c r="E193" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="194" spans="1:1">
-      <c r="A194" s="1"/>
+      <c r="A194" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B194" t="s">
+        <v>105</v>
+      </c>
+      <c r="C194" t="s">
+        <v>11</v>
+      </c>
+      <c r="D194" t="s">
+        <v>12</v>
+      </c>
+      <c r="E194" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="195" spans="1:1">
-      <c r="A195" s="1"/>
+      <c r="A195" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B195" t="s">
+        <v>107</v>
+      </c>
+      <c r="C195" t="s">
+        <v>11</v>
+      </c>
+      <c r="D195" t="s">
+        <v>12</v>
+      </c>
+      <c r="E195" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="1"/>
+      <c r="A196" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B196" t="s">
+        <v>108</v>
+      </c>
+      <c r="C196" t="s">
+        <v>11</v>
+      </c>
+      <c r="D196" t="s">
+        <v>12</v>
+      </c>
+      <c r="E196" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="1"/>
+      <c r="A197" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B197" t="s">
+        <v>110</v>
+      </c>
+      <c r="C197" t="s">
+        <v>11</v>
+      </c>
+      <c r="D197" t="s">
+        <v>12</v>
+      </c>
+      <c r="E197" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="1"/>
+      <c r="A198" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B198" t="s">
+        <v>111</v>
+      </c>
+      <c r="C198" t="s">
+        <v>11</v>
+      </c>
+      <c r="D198" t="s">
+        <v>12</v>
+      </c>
+      <c r="E198" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="1"/>
+      <c r="A199" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B199" t="s">
+        <v>112</v>
+      </c>
+      <c r="C199" t="s">
+        <v>11</v>
+      </c>
+      <c r="D199" t="s">
+        <v>12</v>
+      </c>
+      <c r="E199" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="1"/>
+      <c r="A200" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B200" t="s">
+        <v>113</v>
+      </c>
+      <c r="C200" t="s">
+        <v>11</v>
+      </c>
+      <c r="D200" t="s">
+        <v>12</v>
+      </c>
+      <c r="E200" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="1"/>
+      <c r="A201" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B201" t="s">
+        <v>114</v>
+      </c>
+      <c r="C201" t="s">
+        <v>11</v>
+      </c>
+      <c r="D201" t="s">
+        <v>12</v>
+      </c>
+      <c r="E201" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="1"/>
+      <c r="A202" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B202" t="s">
+        <v>116</v>
+      </c>
+      <c r="C202" t="s">
+        <v>11</v>
+      </c>
+      <c r="D202" t="s">
+        <v>12</v>
+      </c>
+      <c r="E202" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="1"/>
+      <c r="A203" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B203" t="s">
+        <v>117</v>
+      </c>
+      <c r="C203" t="s">
+        <v>11</v>
+      </c>
+      <c r="D203" t="s">
+        <v>12</v>
+      </c>
+      <c r="E203" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="204" spans="1:1">
-      <c r="A204" s="1"/>
+      <c r="A204" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B204" t="s">
+        <v>118</v>
+      </c>
+      <c r="C204" t="s">
+        <v>11</v>
+      </c>
+      <c r="D204" t="s">
+        <v>12</v>
+      </c>
+      <c r="E204" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="205" spans="1:1">
-      <c r="A205" s="1"/>
+      <c r="A205" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B205" t="s">
+        <v>120</v>
+      </c>
+      <c r="C205" t="s">
+        <v>12</v>
+      </c>
+      <c r="D205" t="s">
+        <v>67</v>
+      </c>
+      <c r="E205" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="206" spans="1:1">
-      <c r="A206" s="1"/>
+      <c r="A206" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B206" t="s">
+        <v>121</v>
+      </c>
+      <c r="C206" t="s">
+        <v>12</v>
+      </c>
+      <c r="D206" t="s">
+        <v>12</v>
+      </c>
+      <c r="E206" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="207" spans="1:1">
-      <c r="A207" s="1"/>
+      <c r="A207" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B207" t="s">
+        <v>123</v>
+      </c>
+      <c r="C207" t="s">
+        <v>11</v>
+      </c>
+      <c r="D207" t="s">
+        <v>12</v>
+      </c>
+      <c r="E207" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208" s="1"/>
+      <c r="A208" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B208" t="s">
+        <v>124</v>
+      </c>
+      <c r="C208" t="s">
+        <v>11</v>
+      </c>
+      <c r="D208" t="s">
+        <v>12</v>
+      </c>
+      <c r="E208" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="209" spans="1:1">
-      <c r="A209" s="1"/>
+      <c r="A209" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B209" t="s">
+        <v>125</v>
+      </c>
+      <c r="C209" t="s">
+        <v>12</v>
+      </c>
+      <c r="D209" t="s">
+        <v>12</v>
+      </c>
+      <c r="E209" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" s="1"/>
+      <c r="A210" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B210" t="s">
+        <v>127</v>
+      </c>
+      <c r="C210" t="s">
+        <v>11</v>
+      </c>
+      <c r="D210" t="s">
+        <v>12</v>
+      </c>
+      <c r="E210" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="211" spans="1:1">
-      <c r="A211" s="1"/>
+      <c r="A211" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B211" t="s">
+        <v>128</v>
+      </c>
+      <c r="C211" t="s">
+        <v>11</v>
+      </c>
+      <c r="D211" t="s">
+        <v>13</v>
+      </c>
+      <c r="E211" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212" s="1"/>
+      <c r="A212" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B212" t="s">
+        <v>129</v>
+      </c>
+      <c r="C212" t="s">
+        <v>11</v>
+      </c>
+      <c r="D212" t="s">
+        <v>12</v>
+      </c>
+      <c r="E212" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>126</v>
+      </c>
+      <c r="B213" t="s">
+        <v>130</v>
+      </c>
+      <c r="C213" t="s">
+        <v>11</v>
+      </c>
+      <c r="D213" t="s">
+        <v>12</v>
+      </c>
+      <c r="E213" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>131</v>
+      </c>
+      <c r="B214" t="s">
+        <v>132</v>
+      </c>
+      <c r="C214" t="s">
+        <v>12</v>
+      </c>
+      <c r="D214" t="s">
+        <v>12</v>
+      </c>
+      <c r="E214" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>190</v>
+      </c>
+      <c r="B215" t="s">
+        <v>133</v>
+      </c>
+      <c r="C215" t="s">
+        <v>11</v>
+      </c>
+      <c r="D215" t="s">
+        <v>12</v>
+      </c>
+      <c r="E215" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>131</v>
+      </c>
+      <c r="B216" t="s">
+        <v>134</v>
+      </c>
+      <c r="C216" t="s">
+        <v>11</v>
+      </c>
+      <c r="D216" t="s">
+        <v>12</v>
+      </c>
+      <c r="E216" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>190</v>
+      </c>
+      <c r="B217" t="s">
+        <v>135</v>
+      </c>
+      <c r="C217" t="s">
+        <v>11</v>
+      </c>
+      <c r="D217" t="s">
+        <v>12</v>
+      </c>
+      <c r="E217" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>137</v>
+      </c>
+      <c r="B218" t="s">
+        <v>138</v>
+      </c>
+      <c r="C218" t="s">
+        <v>11</v>
+      </c>
+      <c r="D218" t="s">
+        <v>13</v>
+      </c>
+      <c r="E218" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>137</v>
+      </c>
+      <c r="B219" t="s">
+        <v>139</v>
+      </c>
+      <c r="C219" t="s">
+        <v>12</v>
+      </c>
+      <c r="D219" t="s">
+        <v>13</v>
+      </c>
+      <c r="E219" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>137</v>
+      </c>
+      <c r="B220" t="s">
+        <v>140</v>
+      </c>
+      <c r="C220" t="s">
+        <v>12</v>
+      </c>
+      <c r="D220" t="s">
+        <v>12</v>
+      </c>
+      <c r="E220" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>141</v>
+      </c>
+      <c r="B221" t="s">
+        <v>142</v>
+      </c>
+      <c r="C221" t="s">
+        <v>11</v>
+      </c>
+      <c r="D221" t="s">
+        <v>12</v>
+      </c>
+      <c r="E221" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>141</v>
+      </c>
+      <c r="B222" t="s">
+        <v>143</v>
+      </c>
+      <c r="C222" t="s">
+        <v>11</v>
+      </c>
+      <c r="D222" t="s">
+        <v>12</v>
+      </c>
+      <c r="E222" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>141</v>
+      </c>
+      <c r="B223" t="s">
+        <v>144</v>
+      </c>
+      <c r="C223" t="s">
+        <v>11</v>
+      </c>
+      <c r="D223" t="s">
+        <v>12</v>
+      </c>
+      <c r="E223" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>141</v>
+      </c>
+      <c r="B224" t="s">
+        <v>145</v>
+      </c>
+      <c r="C224" t="s">
+        <v>11</v>
+      </c>
+      <c r="D224" t="s">
+        <v>12</v>
+      </c>
+      <c r="E224" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>141</v>
+      </c>
+      <c r="B225" t="s">
+        <v>146</v>
+      </c>
+      <c r="C225" t="s">
+        <v>11</v>
+      </c>
+      <c r="D225" t="s">
+        <v>12</v>
+      </c>
+      <c r="E225" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>141</v>
+      </c>
+      <c r="B226" t="s">
+        <v>147</v>
+      </c>
+      <c r="C226" t="s">
+        <v>12</v>
+      </c>
+      <c r="D226" t="s">
+        <v>12</v>
+      </c>
+      <c r="E226" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>148</v>
+      </c>
+      <c r="B227" t="s">
+        <v>149</v>
+      </c>
+      <c r="C227" t="s">
+        <v>12</v>
+      </c>
+      <c r="D227" t="s">
+        <v>13</v>
+      </c>
+      <c r="E227" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>150</v>
+      </c>
+      <c r="B228" t="s">
+        <v>151</v>
+      </c>
+      <c r="C228" t="s">
+        <v>12</v>
+      </c>
+      <c r="D228" t="s">
+        <v>12</v>
+      </c>
+      <c r="E228" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>150</v>
+      </c>
+      <c r="B229" t="s">
+        <v>152</v>
+      </c>
+      <c r="C229" t="s">
+        <v>11</v>
+      </c>
+      <c r="D229" t="s">
+        <v>12</v>
+      </c>
+      <c r="E229" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>150</v>
+      </c>
+      <c r="B230" t="s">
+        <v>153</v>
+      </c>
+      <c r="C230" t="s">
+        <v>11</v>
+      </c>
+      <c r="D230" t="s">
+        <v>12</v>
+      </c>
+      <c r="E230" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>150</v>
+      </c>
+      <c r="B231" t="s">
+        <v>154</v>
+      </c>
+      <c r="C231" t="s">
+        <v>11</v>
+      </c>
+      <c r="D231" t="s">
+        <v>12</v>
+      </c>
+      <c r="E231" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>155</v>
+      </c>
+      <c r="B232" t="s">
+        <v>156</v>
+      </c>
+      <c r="C232" t="s">
+        <v>11</v>
+      </c>
+      <c r="D232" t="s">
+        <v>13</v>
+      </c>
+      <c r="E232" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>155</v>
+      </c>
+      <c r="B233" t="s">
+        <v>157</v>
+      </c>
+      <c r="C233" t="s">
+        <v>12</v>
+      </c>
+      <c r="D233" t="s">
+        <v>13</v>
+      </c>
+      <c r="E233" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>155</v>
+      </c>
+      <c r="B234" t="s">
+        <v>158</v>
+      </c>
+      <c r="C234" t="s">
+        <v>11</v>
+      </c>
+      <c r="D234" t="s">
+        <v>12</v>
+      </c>
+      <c r="E234" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>155</v>
+      </c>
+      <c r="B235" t="s">
+        <v>159</v>
+      </c>
+      <c r="C235" t="s">
+        <v>12</v>
+      </c>
+      <c r="D235" t="s">
+        <v>13</v>
+      </c>
+      <c r="E235" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>160</v>
+      </c>
+      <c r="B236" t="s">
+        <v>161</v>
+      </c>
+      <c r="C236" t="s">
+        <v>11</v>
+      </c>
+      <c r="D236" t="s">
+        <v>12</v>
+      </c>
+      <c r="E236" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>160</v>
+      </c>
+      <c r="B237" t="s">
+        <v>162</v>
+      </c>
+      <c r="C237" t="s">
+        <v>11</v>
+      </c>
+      <c r="D237" t="s">
+        <v>12</v>
+      </c>
+      <c r="E237" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>160</v>
+      </c>
+      <c r="B238" t="s">
+        <v>163</v>
+      </c>
+      <c r="C238" t="s">
+        <v>12</v>
+      </c>
+      <c r="D238" t="s">
+        <v>13</v>
+      </c>
+      <c r="E238" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>164</v>
+      </c>
+      <c r="B239" t="s">
+        <v>165</v>
+      </c>
+      <c r="C239" t="s">
+        <v>12</v>
+      </c>
+      <c r="D239" t="s">
+        <v>12</v>
+      </c>
+      <c r="E239" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>164</v>
+      </c>
+      <c r="B240" t="s">
+        <v>166</v>
+      </c>
+      <c r="C240" t="s">
+        <v>11</v>
+      </c>
+      <c r="D240" t="s">
+        <v>12</v>
+      </c>
+      <c r="E240" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>164</v>
+      </c>
+      <c r="B241" t="s">
+        <v>167</v>
+      </c>
+      <c r="C241" t="s">
+        <v>12</v>
+      </c>
+      <c r="D241" t="s">
+        <v>13</v>
+      </c>
+      <c r="E241" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>164</v>
+      </c>
+      <c r="B242" t="s">
+        <v>168</v>
+      </c>
+      <c r="C242" t="s">
+        <v>11</v>
+      </c>
+      <c r="D242" t="s">
+        <v>12</v>
+      </c>
+      <c r="E242" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>169</v>
+      </c>
+      <c r="B243" t="s">
+        <v>170</v>
+      </c>
+      <c r="C243" t="s">
+        <v>11</v>
+      </c>
+      <c r="D243" t="s">
+        <v>12</v>
+      </c>
+      <c r="E243" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>169</v>
+      </c>
+      <c r="B244" t="s">
+        <v>171</v>
+      </c>
+      <c r="C244" t="s">
+        <v>11</v>
+      </c>
+      <c r="D244" t="s">
+        <v>12</v>
+      </c>
+      <c r="E244" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>169</v>
+      </c>
+      <c r="B245" t="s">
+        <v>172</v>
+      </c>
+      <c r="C245" t="s">
+        <v>12</v>
+      </c>
+      <c r="D245" t="s">
+        <v>13</v>
+      </c>
+      <c r="E245" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>169</v>
+      </c>
+      <c r="B246" t="s">
+        <v>173</v>
+      </c>
+      <c r="C246" t="s">
+        <v>12</v>
+      </c>
+      <c r="D246" t="s">
+        <v>12</v>
+      </c>
+      <c r="E246" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>169</v>
+      </c>
+      <c r="B247" t="s">
+        <v>174</v>
+      </c>
+      <c r="C247" t="s">
+        <v>12</v>
+      </c>
+      <c r="D247" t="s">
+        <v>13</v>
+      </c>
+      <c r="E247" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>175</v>
+      </c>
+      <c r="B248" t="s">
+        <v>176</v>
+      </c>
+      <c r="C248" t="s">
+        <v>12</v>
+      </c>
+      <c r="D248" t="s">
+        <v>12</v>
+      </c>
+      <c r="E248" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>175</v>
+      </c>
+      <c r="B249" t="s">
+        <v>177</v>
+      </c>
+      <c r="C249" t="s">
+        <v>12</v>
+      </c>
+      <c r="D249" t="s">
+        <v>13</v>
+      </c>
+      <c r="E249" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>178</v>
+      </c>
+      <c r="B250" t="s">
+        <v>179</v>
+      </c>
+      <c r="C250" t="s">
+        <v>11</v>
+      </c>
+      <c r="D250" t="s">
+        <v>12</v>
+      </c>
+      <c r="E250" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>178</v>
+      </c>
+      <c r="B251" t="s">
+        <v>180</v>
+      </c>
+      <c r="C251" t="s">
+        <v>11</v>
+      </c>
+      <c r="D251" t="s">
+        <v>13</v>
+      </c>
+      <c r="E251" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>178</v>
+      </c>
+      <c r="B252" t="s">
+        <v>181</v>
+      </c>
+      <c r="C252" t="s">
+        <v>11</v>
+      </c>
+      <c r="D252" t="s">
+        <v>13</v>
+      </c>
+      <c r="E252" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>178</v>
+      </c>
+      <c r="B253" t="s">
+        <v>182</v>
+      </c>
+      <c r="C253" t="s">
+        <v>12</v>
+      </c>
+      <c r="D253" t="s">
+        <v>13</v>
+      </c>
+      <c r="E253" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>183</v>
+      </c>
+      <c r="B254" t="s">
+        <v>184</v>
+      </c>
+      <c r="C254" t="s">
+        <v>11</v>
+      </c>
+      <c r="D254" t="s">
+        <v>12</v>
+      </c>
+      <c r="E254" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>185</v>
+      </c>
+      <c r="B255" t="s">
+        <v>186</v>
+      </c>
+      <c r="C255" t="s">
+        <v>12</v>
+      </c>
+      <c r="D255" t="s">
+        <v>13</v>
+      </c>
+      <c r="E255" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>185</v>
+      </c>
+      <c r="B256" t="s">
+        <v>187</v>
+      </c>
+      <c r="C256" t="s">
+        <v>11</v>
+      </c>
+      <c r="D256" t="s">
+        <v>12</v>
+      </c>
+      <c r="E256" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>185</v>
+      </c>
+      <c r="B257" t="s">
+        <v>188</v>
+      </c>
+      <c r="C257" t="s">
+        <v>11</v>
+      </c>
+      <c r="D257" t="s">
+        <v>12</v>
+      </c>
+      <c r="E257" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>185</v>
+      </c>
+      <c r="B258" t="s">
+        <v>189</v>
+      </c>
+      <c r="C258" t="s">
+        <v>12</v>
+      </c>
+      <c r="D258" t="s">
+        <v>13</v>
+      </c>
+      <c r="E258" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>190</v>
+      </c>
+      <c r="B259" t="s">
+        <v>191</v>
+      </c>
+      <c r="C259" t="s">
+        <v>12</v>
+      </c>
+      <c r="D259" t="s">
+        <v>13</v>
+      </c>
+      <c r="E259" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>192</v>
+      </c>
+      <c r="B260" t="s">
+        <v>193</v>
+      </c>
+      <c r="C260" t="s">
+        <v>11</v>
+      </c>
+      <c r="D260" t="s">
+        <v>12</v>
+      </c>
+      <c r="E260" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>192</v>
+      </c>
+      <c r="B261" t="s">
+        <v>194</v>
+      </c>
+      <c r="C261" t="s">
+        <v>11</v>
+      </c>
+      <c r="D261" t="s">
+        <v>12</v>
+      </c>
+      <c r="E261" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>192</v>
+      </c>
+      <c r="B262" t="s">
+        <v>195</v>
+      </c>
+      <c r="C262" t="s">
+        <v>11</v>
+      </c>
+      <c r="D262" t="s">
+        <v>13</v>
+      </c>
+      <c r="E262" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>196</v>
+      </c>
+      <c r="B263" t="s">
+        <v>197</v>
+      </c>
+      <c r="C263" t="s">
+        <v>12</v>
+      </c>
+      <c r="D263" t="s">
+        <v>13</v>
+      </c>
+      <c r="E263" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>198</v>
+      </c>
+      <c r="B264" t="s">
+        <v>199</v>
+      </c>
+      <c r="C264" t="s">
+        <v>11</v>
+      </c>
+      <c r="D264" t="s">
+        <v>13</v>
+      </c>
+      <c r="E264" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>198</v>
+      </c>
+      <c r="B265" t="s">
+        <v>200</v>
+      </c>
+      <c r="C265" t="s">
+        <v>11</v>
+      </c>
+      <c r="D265" t="s">
+        <v>12</v>
+      </c>
+      <c r="E265" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>201</v>
+      </c>
+      <c r="B266" t="s">
+        <v>202</v>
+      </c>
+      <c r="C266" t="s">
+        <v>12</v>
+      </c>
+      <c r="D266" t="s">
+        <v>67</v>
+      </c>
+      <c r="E266" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>201</v>
+      </c>
+      <c r="B267" t="s">
+        <v>203</v>
+      </c>
+      <c r="C267" t="s">
+        <v>11</v>
+      </c>
+      <c r="D267" t="s">
+        <v>12</v>
+      </c>
+      <c r="E267" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>201</v>
+      </c>
+      <c r="B268" t="s">
+        <v>204</v>
+      </c>
+      <c r="C268" t="s">
+        <v>11</v>
+      </c>
+      <c r="D268" t="s">
+        <v>13</v>
+      </c>
+      <c r="E268" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>205</v>
+      </c>
+      <c r="B269" t="s">
+        <v>206</v>
+      </c>
+      <c r="C269" t="s">
+        <v>12</v>
+      </c>
+      <c r="D269" t="s">
+        <v>13</v>
+      </c>
+      <c r="E269" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>205</v>
+      </c>
+      <c r="B270" t="s">
+        <v>207</v>
+      </c>
+      <c r="C270" t="s">
+        <v>11</v>
+      </c>
+      <c r="D270" t="s">
+        <v>13</v>
+      </c>
+      <c r="E270" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>205</v>
+      </c>
+      <c r="B271" t="s">
+        <v>208</v>
+      </c>
+      <c r="C271" t="s">
+        <v>11</v>
+      </c>
+      <c r="D271" t="s">
+        <v>12</v>
+      </c>
+      <c r="E271" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>209</v>
+      </c>
+      <c r="B272" t="s">
+        <v>210</v>
+      </c>
+      <c r="C272" t="s">
+        <v>11</v>
+      </c>
+      <c r="D272" t="s">
+        <v>13</v>
+      </c>
+      <c r="E272" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>209</v>
+      </c>
+      <c r="B273" t="s">
+        <v>211</v>
+      </c>
+      <c r="C273" t="s">
+        <v>11</v>
+      </c>
+      <c r="D273" t="s">
+        <v>13</v>
+      </c>
+      <c r="E273" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>213</v>
+      </c>
+      <c r="B274" t="s">
+        <v>214</v>
+      </c>
+      <c r="C274" t="s">
+        <v>12</v>
+      </c>
+      <c r="D274" t="s">
+        <v>13</v>
+      </c>
+      <c r="E274" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>215</v>
+      </c>
+      <c r="B275" t="s">
+        <v>216</v>
+      </c>
+      <c r="C275" t="s">
+        <v>12</v>
+      </c>
+      <c r="D275" t="s">
+        <v>13</v>
+      </c>
+      <c r="E275" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>215</v>
+      </c>
+      <c r="B276" t="s">
+        <v>217</v>
+      </c>
+      <c r="C276" t="s">
+        <v>11</v>
+      </c>
+      <c r="D276" t="s">
+        <v>12</v>
+      </c>
+      <c r="E276" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>218</v>
+      </c>
+      <c r="B277" t="s">
+        <v>219</v>
+      </c>
+      <c r="C277" t="s">
+        <v>12</v>
+      </c>
+      <c r="D277" t="s">
+        <v>12</v>
+      </c>
+      <c r="E277" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
+        <v>218</v>
+      </c>
+      <c r="B278" t="s">
+        <v>220</v>
+      </c>
+      <c r="C278" t="s">
+        <v>12</v>
+      </c>
+      <c r="D278" t="s">
+        <v>13</v>
+      </c>
+      <c r="E278" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>218</v>
+      </c>
+      <c r="B279" t="s">
+        <v>221</v>
+      </c>
+      <c r="C279" t="s">
+        <v>12</v>
+      </c>
+      <c r="D279" t="s">
+        <v>12</v>
+      </c>
+      <c r="E279" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>222</v>
+      </c>
+      <c r="B280" t="s">
+        <v>223</v>
+      </c>
+      <c r="C280" t="s">
+        <v>11</v>
+      </c>
+      <c r="D280" t="s">
+        <v>13</v>
+      </c>
+      <c r="E280" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>222</v>
+      </c>
+      <c r="B281" t="s">
+        <v>224</v>
+      </c>
+      <c r="C281" t="s">
+        <v>11</v>
+      </c>
+      <c r="D281" t="s">
+        <v>13</v>
+      </c>
+      <c r="E281" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>222</v>
+      </c>
+      <c r="B282" t="s">
+        <v>225</v>
+      </c>
+      <c r="C282" t="s">
+        <v>11</v>
+      </c>
+      <c r="D282" t="s">
+        <v>12</v>
+      </c>
+      <c r="E282" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>222</v>
+      </c>
+      <c r="B283" t="s">
+        <v>226</v>
+      </c>
+      <c r="C283" t="s">
+        <v>11</v>
+      </c>
+      <c r="D283" t="s">
+        <v>12</v>
+      </c>
+      <c r="E283" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>227</v>
+      </c>
+      <c r="B284" t="s">
+        <v>228</v>
+      </c>
+      <c r="C284" t="s">
+        <v>12</v>
+      </c>
+      <c r="D284" t="s">
+        <v>13</v>
+      </c>
+      <c r="E284" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>227</v>
+      </c>
+      <c r="B285" t="s">
+        <v>229</v>
+      </c>
+      <c r="C285" t="s">
+        <v>12</v>
+      </c>
+      <c r="D285" t="s">
+        <v>13</v>
+      </c>
+      <c r="E285" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>231</v>
+      </c>
+      <c r="B286" t="s">
+        <v>232</v>
+      </c>
+      <c r="C286" t="s">
+        <v>12</v>
+      </c>
+      <c r="D286" t="s">
+        <v>13</v>
+      </c>
+      <c r="E286" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>233</v>
+      </c>
+      <c r="B287" t="s">
+        <v>234</v>
+      </c>
+      <c r="C287" t="s">
+        <v>11</v>
+      </c>
+      <c r="D287" t="s">
+        <v>12</v>
+      </c>
+      <c r="E287" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>233</v>
+      </c>
+      <c r="B288" t="s">
+        <v>235</v>
+      </c>
+      <c r="C288" t="s">
+        <v>11</v>
+      </c>
+      <c r="D288" t="s">
+        <v>12</v>
+      </c>
+      <c r="E288" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>233</v>
+      </c>
+      <c r="B289" t="s">
+        <v>236</v>
+      </c>
+      <c r="C289" t="s">
+        <v>11</v>
+      </c>
+      <c r="D289" t="s">
+        <v>12</v>
+      </c>
+      <c r="E289" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>237</v>
+      </c>
+      <c r="B290" t="s">
+        <v>238</v>
+      </c>
+      <c r="C290" t="s">
+        <v>12</v>
+      </c>
+      <c r="D290" t="s">
+        <v>13</v>
+      </c>
+      <c r="E290" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>237</v>
+      </c>
+      <c r="B291" t="s">
+        <v>239</v>
+      </c>
+      <c r="C291" t="s">
+        <v>12</v>
+      </c>
+      <c r="D291" t="s">
+        <v>13</v>
+      </c>
+      <c r="E291" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>240</v>
+      </c>
+      <c r="B292" t="s">
+        <v>241</v>
+      </c>
+      <c r="C292" t="s">
+        <v>12</v>
+      </c>
+      <c r="D292" t="s">
+        <v>13</v>
+      </c>
+      <c r="E292" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>242</v>
+      </c>
+      <c r="B293" t="s">
+        <v>243</v>
+      </c>
+      <c r="C293" t="s">
+        <v>11</v>
+      </c>
+      <c r="D293" t="s">
+        <v>12</v>
+      </c>
+      <c r="E293" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>242</v>
+      </c>
+      <c r="B294" t="s">
+        <v>244</v>
+      </c>
+      <c r="C294" t="s">
+        <v>12</v>
+      </c>
+      <c r="D294" t="s">
+        <v>12</v>
+      </c>
+      <c r="E294" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>245</v>
+      </c>
+      <c r="B295" t="s">
+        <v>246</v>
+      </c>
+      <c r="C295" t="s">
+        <v>11</v>
+      </c>
+      <c r="D295" t="s">
+        <v>12</v>
+      </c>
+      <c r="E295" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>245</v>
+      </c>
+      <c r="B296" t="s">
+        <v>247</v>
+      </c>
+      <c r="C296" t="s">
+        <v>11</v>
+      </c>
+      <c r="D296" t="s">
+        <v>12</v>
+      </c>
+      <c r="E296" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>248</v>
+      </c>
+      <c r="B297" t="s">
+        <v>249</v>
+      </c>
+      <c r="C297" t="s">
+        <v>12</v>
+      </c>
+      <c r="D297" t="s">
+        <v>13</v>
+      </c>
+      <c r="E297" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>248</v>
+      </c>
+      <c r="B298" t="s">
+        <v>250</v>
+      </c>
+      <c r="C298" t="s">
+        <v>12</v>
+      </c>
+      <c r="D298" t="s">
+        <v>13</v>
+      </c>
+      <c r="E298" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>251</v>
+      </c>
+      <c r="B299" t="s">
+        <v>252</v>
+      </c>
+      <c r="C299" t="s">
+        <v>11</v>
+      </c>
+      <c r="D299" t="s">
+        <v>12</v>
+      </c>
+      <c r="E299" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>253</v>
+      </c>
+      <c r="B300" t="s">
+        <v>254</v>
+      </c>
+      <c r="C300" t="s">
+        <v>11</v>
+      </c>
+      <c r="D300" t="s">
+        <v>13</v>
+      </c>
+      <c r="E300" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>253</v>
+      </c>
+      <c r="B301" t="s">
+        <v>255</v>
+      </c>
+      <c r="C301" t="s">
+        <v>12</v>
+      </c>
+      <c r="D301" t="s">
+        <v>13</v>
+      </c>
+      <c r="E301" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>256</v>
+      </c>
+      <c r="B302" t="s">
+        <v>257</v>
+      </c>
+      <c r="C302" t="s">
+        <v>11</v>
+      </c>
+      <c r="D302" t="s">
+        <v>12</v>
+      </c>
+      <c r="E302" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>256</v>
+      </c>
+      <c r="B303" t="s">
+        <v>258</v>
+      </c>
+      <c r="C303" t="s">
+        <v>11</v>
+      </c>
+      <c r="D303" t="s">
+        <v>12</v>
+      </c>
+      <c r="E303" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>256</v>
+      </c>
+      <c r="B304" t="s">
+        <v>259</v>
+      </c>
+      <c r="C304" t="s">
+        <v>11</v>
+      </c>
+      <c r="D304" t="s">
+        <v>12</v>
+      </c>
+      <c r="E304" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>260</v>
+      </c>
+      <c r="B305" t="s">
+        <v>261</v>
+      </c>
+      <c r="C305" t="s">
+        <v>11</v>
+      </c>
+      <c r="D305" t="s">
+        <v>12</v>
+      </c>
+      <c r="E305" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>260</v>
+      </c>
+      <c r="B306" t="s">
+        <v>262</v>
+      </c>
+      <c r="C306" t="s">
+        <v>12</v>
+      </c>
+      <c r="D306" t="s">
+        <v>12</v>
+      </c>
+      <c r="E306" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>